<commit_message>
LocalTestTwo runs ok both on localhost and remote server
</commit_message>
<xml_diff>
--- a/resources/LocalTestData.xlsx
+++ b/resources/LocalTestData.xlsx
@@ -195,9 +195,6 @@
     <t>testFirstName1</t>
   </si>
   <si>
-    <t>testLadtName1</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -207,72 +204,48 @@
     <t>testFirstName2</t>
   </si>
   <si>
-    <t>testLadtName2</t>
-  </si>
-  <si>
     <t>Comment2</t>
   </si>
   <si>
     <t>testFirstName3</t>
   </si>
   <si>
-    <t>testLadtName3</t>
-  </si>
-  <si>
     <t>Comment3</t>
   </si>
   <si>
     <t>testFirstName4</t>
   </si>
   <si>
-    <t>testLadtName4</t>
-  </si>
-  <si>
     <t>Comment4</t>
   </si>
   <si>
     <t>testFirstName5</t>
   </si>
   <si>
-    <t>testLadtName5</t>
-  </si>
-  <si>
     <t>Comment5</t>
   </si>
   <si>
     <t>testFirstName6</t>
   </si>
   <si>
-    <t>testLadtName6</t>
-  </si>
-  <si>
     <t>Comment6</t>
   </si>
   <si>
     <t>testFirstName7</t>
   </si>
   <si>
-    <t>testLadtName7</t>
-  </si>
-  <si>
     <t>Comment7</t>
   </si>
   <si>
     <t>testFirstName8</t>
   </si>
   <si>
-    <t>testLadtName8</t>
-  </si>
-  <si>
     <t>Comment8</t>
   </si>
   <si>
     <t>testFirstName9</t>
   </si>
   <si>
-    <t>testLadtName9</t>
-  </si>
-  <si>
     <t>Comment9</t>
   </si>
   <si>
@@ -301,6 +274,33 @@
   </si>
   <si>
     <t>test9@test.com</t>
+  </si>
+  <si>
+    <t>testLastName1</t>
+  </si>
+  <si>
+    <t>testLastName2</t>
+  </si>
+  <si>
+    <t>testLastName3</t>
+  </si>
+  <si>
+    <t>testLastName4</t>
+  </si>
+  <si>
+    <t>testLastName5</t>
+  </si>
+  <si>
+    <t>testLastName6</t>
+  </si>
+  <si>
+    <t>testLastName7</t>
+  </si>
+  <si>
+    <t>testLastName8</t>
+  </si>
+  <si>
+    <t>testLastName9</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M9"/>
+      <selection activeCell="L1" sqref="L1:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,16 +705,16 @@
         <v>58</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -749,19 +749,19 @@
         <v>57</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -792,19 +792,19 @@
         <v>57</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -839,19 +839,19 @@
         <v>57</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -886,19 +886,19 @@
         <v>57</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -929,19 +929,19 @@
         <v>57</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -976,19 +976,19 @@
         <v>57</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1023,19 +1023,19 @@
         <v>57</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1066,19 +1066,19 @@
         <v>57</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExcelUtils fixed from 1,1 Remote Platforms changed
</commit_message>
<xml_diff>
--- a/resources/LocalTestData.xlsx
+++ b/resources/LocalTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
   <si>
     <t>50.01</t>
   </si>
@@ -301,6 +301,54 @@
   </si>
   <si>
     <t>testLastName9</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -346,7 +394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -359,9 +407,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,7 +447,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -471,7 +519,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -645,447 +693,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="17" style="1"/>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="1" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>